<commit_message>
ci: update age issue
</commit_message>
<xml_diff>
--- a/LF/Confirmation/Cote d'Ivoire/ci_202302_lf_conf_3_fts_result.xlsx
+++ b/LF/Confirmation/Cote d'Ivoire/ci_202302_lf_conf_3_fts_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositories\WHO\dsa-forms\LF\Confirmation\Cote d'Ivoire\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228CA635-F34D-40A4-A5D8-FD205E7F6450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886D99F6-A2A5-4769-A0FF-72694702F863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -246,15 +246,6 @@
     <t>Entrer l'âge du participant (en années)</t>
   </si>
   <si>
-    <t>. &gt;= 5 and . &lt;= 9</t>
-  </si>
-  <si>
-    <t>The age must be between 5 and 9 years</t>
-  </si>
-  <si>
-    <t>L'age doit être compris entre 5 et 9 ans</t>
-  </si>
-  <si>
     <t>d_lotnumber1</t>
   </si>
   <si>
@@ -612,6 +603,15 @@
   </si>
   <si>
     <t>(2023 Fev) 3. Recartographie FL - Résultat FTS</t>
+  </si>
+  <si>
+    <t>. &gt;= 1 and . &lt;= 120</t>
+  </si>
+  <si>
+    <t>Please enter a valide age</t>
+  </si>
+  <si>
+    <t>Veuillez entrer un age valide.</t>
   </si>
 </sst>
 </file>
@@ -1129,11 +1129,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1251,7 +1251,7 @@
         <v>27</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>28</v>
@@ -1538,7 +1538,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:17" s="3" customFormat="1" ht="31.5">
+    <row r="13" spans="1:17" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1555,13 +1555,13 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="3" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>76</v>
+        <v>192</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -1577,14 +1577,14 @@
         <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F14" s="31"/>
       <c r="G14" s="17"/>
@@ -1602,22 +1602,22 @@
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" ht="31.5">
       <c r="A15" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="E15" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="F15" s="31" t="s">
         <v>82</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>85</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -1634,17 +1634,17 @@
     </row>
     <row r="16" spans="1:17" s="3" customFormat="1">
       <c r="A16" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F16" s="31"/>
       <c r="G16" s="17"/>
@@ -1652,7 +1652,7 @@
       <c r="I16" s="23"/>
       <c r="J16" s="31"/>
       <c r="K16" s="5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L16" s="5"/>
       <c r="M16" s="17" t="s">
@@ -1664,17 +1664,17 @@
     </row>
     <row r="17" spans="1:16" s="3" customFormat="1">
       <c r="A17" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F17" s="31"/>
       <c r="G17" s="17"/>
@@ -1682,7 +1682,7 @@
       <c r="I17" s="23"/>
       <c r="J17" s="31"/>
       <c r="K17" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L17" s="5"/>
       <c r="M17" s="17" t="s">
@@ -1694,10 +1694,10 @@
     </row>
     <row r="18" spans="1:16" s="3" customFormat="1">
       <c r="A18" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
@@ -1709,7 +1709,7 @@
       <c r="J18" s="31"/>
       <c r="K18" s="5"/>
       <c r="L18" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="M18" s="17" t="s">
         <v>26</v>
@@ -1720,17 +1720,17 @@
     </row>
     <row r="19" spans="1:16" s="3" customFormat="1">
       <c r="A19" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F19" s="31"/>
       <c r="G19" s="17"/>
@@ -1738,7 +1738,7 @@
       <c r="I19" s="23"/>
       <c r="J19" s="31"/>
       <c r="K19" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L19" s="17"/>
       <c r="M19" s="17" t="s">
@@ -1750,17 +1750,17 @@
     </row>
     <row r="20" spans="1:16" s="3" customFormat="1" ht="63">
       <c r="A20" s="17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="28" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F20" s="31"/>
       <c r="G20" s="17"/>
@@ -1768,7 +1768,7 @@
       <c r="I20" s="23"/>
       <c r="J20" s="31"/>
       <c r="K20" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
@@ -1781,14 +1781,14 @@
         <v>27</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="17"/>
@@ -1796,7 +1796,7 @@
       <c r="I21" s="23"/>
       <c r="J21" s="31"/>
       <c r="K21" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L21" s="17"/>
       <c r="M21" s="17" t="s">
@@ -1808,29 +1808,29 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="E22" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="7"/>
       <c r="J22" s="8"/>
       <c r="K22" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L22" s="6"/>
       <c r="M22" s="17" t="s">
@@ -1842,17 +1842,17 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C23" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="6"/>
@@ -1860,7 +1860,7 @@
       <c r="I23" s="7"/>
       <c r="J23" s="8"/>
       <c r="K23" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="17" t="s">
@@ -1872,17 +1872,17 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="6"/>
@@ -1890,7 +1890,7 @@
       <c r="I24" s="7"/>
       <c r="J24" s="8"/>
       <c r="K24" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="17" t="s">
@@ -1902,10 +1902,10 @@
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="7"/>
@@ -1916,10 +1916,10 @@
       <c r="I25" s="7"/>
       <c r="J25" s="8"/>
       <c r="K25" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
@@ -1928,10 +1928,10 @@
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1943,7 +1943,7 @@
       <c r="J26" s="8"/>
       <c r="K26" s="17"/>
       <c r="L26" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
@@ -1952,17 +1952,17 @@
     </row>
     <row r="27" spans="1:16" s="14" customFormat="1">
       <c r="A27" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="32" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F27" s="32"/>
       <c r="G27" s="25"/>
@@ -1978,17 +1978,17 @@
     </row>
     <row r="28" spans="1:16" s="3" customFormat="1">
       <c r="A28" s="17" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="28" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F28" s="31"/>
       <c r="G28" s="17"/>
@@ -1996,7 +1996,7 @@
       <c r="I28" s="23"/>
       <c r="J28" s="31"/>
       <c r="K28" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="L28" s="17"/>
       <c r="M28" s="17" t="s">
@@ -2011,14 +2011,14 @@
         <v>27</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C29" s="24" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="6"/>
@@ -2026,7 +2026,7 @@
       <c r="I29" s="7"/>
       <c r="J29" s="8"/>
       <c r="K29" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L29" s="6"/>
       <c r="M29" s="6"/>
@@ -2036,17 +2036,17 @@
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="17" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="6"/>
@@ -2062,10 +2062,10 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="17" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="7"/>
@@ -2084,10 +2084,10 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="17" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="7"/>
@@ -2129,7 +2129,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2141,237 +2141,237 @@
         <v>4</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B3" t="s">
         <v>140</v>
       </c>
-      <c r="B3" t="s">
-        <v>143</v>
-      </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" t="s">
         <v>145</v>
       </c>
-      <c r="B5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>148</v>
-      </c>
       <c r="D5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" t="s">
         <v>150</v>
       </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D9" t="s">
         <v>158</v>
-      </c>
-      <c r="B9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" t="s">
-        <v>160</v>
-      </c>
-      <c r="D9" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D10" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B11" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B13" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C14" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>183</v>
-      </c>
       <c r="C17" s="7" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -8941,7 +8941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -8953,24 +8953,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="35" customFormat="1">
       <c r="A2" s="21" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>